<commit_message>
updates in preparation for v1.0.0 release
Updates in
- source md files
- reference numbers in the spreadsheet files
- tables that show the version history of spreadsheet files
- sushi-config to indicate the next planned release
</commit_message>
<xml_diff>
--- a/input/dictionary/IMMZ DAK_core data dictionary.xlsx
+++ b/input/dictionary/IMMZ DAK_core data dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WHO\GitHub\smart-dak-immunizations\input\dictionary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/DigitalAcceleratorKits/Shared Documents/Immunizations Digital Accelerator Kit/_FINAL spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9321E77B-0038-4365-9AC2-7A3B04C9B6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{9321E77B-0038-4365-9AC2-7A3B04C9B6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BCFB282-6FCC-4C01-8E41-D6ACB59FA47A}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{8719F19C-F96B-4DEF-AD42-B50F1C4AE782}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8719F19C-F96B-4DEF-AD42-B50F1C4AE782}"/>
   </bookViews>
   <sheets>
     <sheet name="COVER" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'IMMZ.C Client registration'!$A$1:$AE$18</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'IMMZ.D Administer vaccine'!$A$1:$AE$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'IMMZ.D Administer vaccine'!$B$1:$B$195</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'IMMZ.I Report generation'!$A$1:$AI$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'IMMZ.Z Vaccine library'!$A$1:$AE$254</definedName>
     <definedName name="Z_82BB2B85_AB68_4EA1_AAA4_60EA4CEA302B_.wvu.FilterData" localSheetId="2" hidden="1">'IMMZ.C Client registration'!$A$1:$AE$18</definedName>
@@ -7819,7 +7819,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">https://smart.who.int/dak-immz/v0.9.9/IMMZ DAK_core data dictionary.xlsx
+    <t xml:space="preserve">https://smart.who.int/dak-immz/v1.0.0/IMMZ DAK_core data dictionary.xlsx
 © World Health Organization 2024. Some rights reserved. This work is available under the
 </t>
   </si>
@@ -13491,7 +13491,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="B1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="13" x14ac:dyDescent="0.25"/>
   <cols>
@@ -14266,11 +14266,11 @@
   </sheetPr>
   <dimension ref="A1:AI18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA4" sqref="AA4"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.26953125" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
@@ -14308,7 +14308,7 @@
     <col min="36" max="16384" width="12.26953125" style="78"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="56" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="56" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>18</v>
       </c>
@@ -15851,11 +15851,11 @@
   </sheetPr>
   <dimension ref="A1:AI195"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
@@ -17543,7 +17543,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:35" s="72" customFormat="1" ht="58" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:35" s="72" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A21" s="66" t="s">
         <v>326</v>
       </c>
@@ -17620,7 +17620,7 @@
       <c r="AH21" s="68"/>
       <c r="AI21" s="91"/>
     </row>
-    <row r="22" spans="1:35" s="64" customFormat="1" ht="58" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:35" s="64" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A22" s="57" t="s">
         <v>326</v>
       </c>
@@ -19977,7 +19977,7 @@
       <c r="AH50" s="59"/>
       <c r="AI50" s="74"/>
     </row>
-    <row r="51" spans="1:35" s="64" customFormat="1" ht="87" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:35" s="64" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
       <c r="A51" s="57" t="s">
         <v>256</v>
       </c>
@@ -25266,7 +25266,7 @@
       <c r="AH117" s="58"/>
       <c r="AI117" s="62"/>
     </row>
-    <row r="118" spans="1:35" s="64" customFormat="1" ht="72.5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:35" s="64" customFormat="1" ht="58" x14ac:dyDescent="0.25">
       <c r="A118" s="57" t="s">
         <v>908</v>
       </c>
@@ -27382,7 +27382,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="145" spans="1:35" s="119" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:35" s="119" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A145" s="57" t="s">
         <v>908</v>
       </c>
@@ -31479,11 +31479,11 @@
   </sheetPr>
   <dimension ref="A1:AI28"/>
   <sheetViews>
-    <sheetView zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
@@ -33607,7 +33607,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y1" sqref="Y1"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.25"/>
@@ -33923,7 +33923,7 @@
       <c r="AK3" s="59"/>
       <c r="AL3" s="74"/>
     </row>
-    <row r="4" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -35987,7 +35987,7 @@
       <c r="AK35" s="59"/>
       <c r="AL35" s="74"/>
     </row>
-    <row r="36" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A36" s="59"/>
       <c r="B36" s="59"/>
       <c r="C36" s="59"/>
@@ -39367,7 +39367,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A88" s="59"/>
       <c r="B88" s="59"/>
       <c r="C88" s="59"/>
@@ -43085,7 +43085,7 @@
       <c r="AK145" s="59"/>
       <c r="AL145" s="74"/>
     </row>
-    <row r="146" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A146" s="59"/>
       <c r="B146" s="59"/>
       <c r="C146" s="59"/>
@@ -43926,7 +43926,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="158" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A158" s="59"/>
       <c r="B158" s="59"/>
       <c r="C158" s="59"/>
@@ -45172,7 +45172,7 @@
       <c r="AK175" s="59"/>
       <c r="AL175" s="74"/>
     </row>
-    <row r="176" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A176" s="59"/>
       <c r="B176" s="59"/>
       <c r="C176" s="59"/>
@@ -45230,7 +45230,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="177" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A177" s="59"/>
       <c r="B177" s="59"/>
       <c r="C177" s="59"/>
@@ -46704,7 +46704,7 @@
       <c r="AK199" s="106"/>
       <c r="AL199" s="106"/>
     </row>
-    <row r="200" spans="1:38" s="105" customFormat="1" ht="101.5" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:38" s="105" customFormat="1" ht="87" x14ac:dyDescent="0.25">
       <c r="A200" s="57" t="s">
         <v>1591</v>
       </c>
@@ -46986,7 +46986,7 @@
       <c r="AK203" s="59"/>
       <c r="AL203" s="74"/>
     </row>
-    <row r="204" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A204" s="59"/>
       <c r="B204" s="59"/>
       <c r="C204" s="59"/>
@@ -47490,7 +47490,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="211" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A211" s="59"/>
       <c r="B211" s="59"/>
       <c r="C211" s="59"/>
@@ -49743,7 +49743,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="245" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A245" s="59"/>
       <c r="B245" s="59"/>
       <c r="C245" s="59"/>
@@ -49802,7 +49802,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="246" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A246" s="59"/>
       <c r="B246" s="59"/>
       <c r="C246" s="59"/>
@@ -50088,7 +50088,7 @@
       <c r="AK250" s="106"/>
       <c r="AL250" s="74"/>
     </row>
-    <row r="251" spans="1:38" s="105" customFormat="1" ht="43.5" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:38" s="105" customFormat="1" ht="29" x14ac:dyDescent="0.25">
       <c r="A251" s="59"/>
       <c r="B251" s="59"/>
       <c r="C251" s="59"/>
@@ -50810,6 +50810,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008A6DDC313EDC9A43B330D8B6305883A5" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a5b0342cd22268e5e5d3683a3cff816e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="73389989-ac93-4f39-a9f3-2949bbf25fcc" xmlns:ns3="51983ca6-de84-41fa-9a65-1d08ee1009bc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c638d06e48d95e9efa3bb75773f50cd7" ns2:_="" ns3:_="">
     <xsd:import namespace="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
@@ -51064,7 +51073,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="51983ca6-de84-41fa-9a65-1d08ee1009bc" xsi:nil="true"/>
@@ -51132,16 +51141,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89F76B6B-9FB5-4EC6-9BBD-29474E3450E0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -51160,21 +51168,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5128250D-9B2C-4D86-9D99-709881CA8B0F}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="51983ca6-de84-41fa-9a65-1d08ee1009bc"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="73389989-ac93-4f39-a9f3-2949bbf25fcc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E3641399-1C83-4230-9FA0-63883702B763}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>